<commit_message>
Report 1, Backlog Update
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -7,13 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="SPRINT1" sheetId="1" r:id="rId1"/>
-    <sheet name="SPRINT2" sheetId="4" r:id="rId2"/>
-    <sheet name="SPRINT3" sheetId="8" r:id="rId3"/>
-    <sheet name="Project Coreflow" sheetId="6" r:id="rId4"/>
-    <sheet name="Question" sheetId="7" r:id="rId5"/>
-    <sheet name="Member" sheetId="2" r:id="rId6"/>
-    <sheet name="TaskStatus" sheetId="3" r:id="rId7"/>
+    <sheet name="Product Backlog" sheetId="10" r:id="rId1"/>
+    <sheet name="SPRINT1" sheetId="1" r:id="rId2"/>
+    <sheet name="SPRINT2" sheetId="4" r:id="rId3"/>
+    <sheet name="SPRINT3" sheetId="8" r:id="rId4"/>
+    <sheet name="Project Coreflow" sheetId="6" r:id="rId5"/>
+    <sheet name="Question" sheetId="7" r:id="rId6"/>
+    <sheet name="Member" sheetId="2" r:id="rId7"/>
+    <sheet name="TaskStatus" sheetId="3" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="Member">Member!$A$1:$A$4</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="75">
   <si>
     <t>No.</t>
   </si>
@@ -146,9 +147,6 @@
     <t>Design main layout</t>
   </si>
   <si>
-    <t>Design login/social network connection UI</t>
-  </si>
-  <si>
     <t>Design Utilities layout</t>
   </si>
   <si>
@@ -163,12 +161,102 @@
   <si>
     <t>ilike</t>
   </si>
+  <si>
+    <t>MOBILE DATING APPS</t>
+  </si>
+  <si>
+    <t>Create User Profile</t>
+  </si>
+  <si>
+    <t>Manage Friends List</t>
+  </si>
+  <si>
+    <t>Realtime chat</t>
+  </si>
+  <si>
+    <t>Register new account</t>
+  </si>
+  <si>
+    <t>Mapping current account and friend list from social network (facebook, google+)</t>
+  </si>
+  <si>
+    <t>Edit profile info: Interest, gender, location,…</t>
+  </si>
+  <si>
+    <t>Modify friend list (unfriends, block..)</t>
+  </si>
+  <si>
+    <t>Scan near-by location  by matching user's interest &amp; profile</t>
+  </si>
+  <si>
+    <t>View profile other people near by you who match your profile</t>
+  </si>
+  <si>
+    <t>Search add new friends</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recommender System </t>
+  </si>
+  <si>
+    <t>Build a recommerder system to suggest friends base on user profile similarity</t>
+  </si>
+  <si>
+    <t>Suggest new friends base on friends connection</t>
+  </si>
+  <si>
+    <t>Suggest user you might want to meet base on your current friend connection</t>
+  </si>
+  <si>
+    <t>Realtime chat, communicate with available friends</t>
+  </si>
+  <si>
+    <t>Receive notification when their friends are near by</t>
+  </si>
+  <si>
+    <t>Chat notification</t>
+  </si>
+  <si>
+    <t>View chat history</t>
+  </si>
+  <si>
+    <t>Design login/social network connection</t>
+  </si>
+  <si>
+    <t>Design setting user profile</t>
+  </si>
+  <si>
+    <t>Design friends list UI</t>
+  </si>
+  <si>
+    <t>Design scan nearby user UI</t>
+  </si>
+  <si>
+    <t>Design UseCase</t>
+  </si>
+  <si>
+    <t>Design ERD</t>
+  </si>
+  <si>
+    <t>Show current location map and display friends which nearby user.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +305,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -332,7 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -396,6 +492,45 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -490,7 +625,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -608,14 +742,12 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>SPRINT1!$B$27:$B$28</c:f>
+              <c:f>SPRINT1!$B$32:$B$33</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -629,7 +761,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SPRINT1!$C$27:$C$28</c:f>
+              <c:f>SPRINT1!$C$32:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -784,7 +916,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -836,7 +967,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>SPRINT1!$B$51:$B$54</c:f>
+              <c:f>SPRINT1!$B$56:$B$59</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -856,7 +987,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SPRINT1!$E$51:$E$54</c:f>
+              <c:f>SPRINT1!$E$56:$E$59</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -886,11 +1017,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="543644352"/>
-        <c:axId val="543644896"/>
+        <c:axId val="1807069408"/>
+        <c:axId val="1807061248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="543644352"/>
+        <c:axId val="1807069408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,7 +1064,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="543644896"/>
+        <c:crossAx val="1807061248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -941,7 +1072,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="543644896"/>
+        <c:axId val="1807061248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -993,7 +1124,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="543644352"/>
+        <c:crossAx val="1807069408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1474,11 +1605,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="695909664"/>
-        <c:axId val="695911296"/>
+        <c:axId val="1958725168"/>
+        <c:axId val="1958719184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="695909664"/>
+        <c:axId val="1958725168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1521,7 +1652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="695911296"/>
+        <c:crossAx val="1958719184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1529,7 +1660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="695911296"/>
+        <c:axId val="1958719184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1581,7 +1712,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="695909664"/>
+        <c:crossAx val="1958725168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2062,11 +2193,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="695904768"/>
-        <c:axId val="695906944"/>
+        <c:axId val="1958720816"/>
+        <c:axId val="1958727344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="695904768"/>
+        <c:axId val="1958720816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2109,7 +2240,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="695906944"/>
+        <c:crossAx val="1958727344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2117,7 +2248,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="695906944"/>
+        <c:axId val="1958727344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2169,7 +2300,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="695904768"/>
+        <c:crossAx val="1958720816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5530,13 +5661,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2609021</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5560,13 +5691,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1190625</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6014,13 +6145,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="35.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="81.5703125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+    </row>
+    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="40">
+        <v>1</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="40"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="40"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="40">
+        <v>2</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="40">
+        <v>3</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="31">
+        <v>4</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
+        <v>5</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="40">
+        <v>6</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="33">
+        <v>7</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6034,11 +6355,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
@@ -6047,52 +6368,52 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
       <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
       <c r="G6" s="16">
         <v>1</v>
       </c>
@@ -6120,19 +6441,21 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" s="7">
         <v>4</v>
       </c>
-      <c r="G7" s="19"/>
+      <c r="G7" s="19">
+        <v>4</v>
+      </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
@@ -6152,16 +6475,14 @@
         <v>5</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F8" s="7">
         <v>16</v>
       </c>
-      <c r="G8" s="19">
-        <v>8</v>
-      </c>
+      <c r="G8" s="19"/>
       <c r="H8" s="19">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
@@ -6174,17 +6495,17 @@
         <v>3</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="7">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
@@ -6199,17 +6520,17 @@
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="7">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -6224,17 +6545,17 @@
         <v>5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="7">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
@@ -6248,18 +6569,18 @@
       <c r="A12" s="7">
         <v>6</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>42</v>
+      <c r="B12" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="7">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
@@ -6273,16 +6594,18 @@
       <c r="A13" s="7">
         <v>7</v>
       </c>
-      <c r="B13" s="30"/>
+      <c r="B13" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="7">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
@@ -6296,7 +6619,9 @@
       <c r="A14" s="7">
         <v>8</v>
       </c>
-      <c r="B14" s="30"/>
+      <c r="B14" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
         <v>7</v>
@@ -6305,7 +6630,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="7">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
@@ -6319,7 +6644,9 @@
       <c r="A15" s="7">
         <v>9</v>
       </c>
-      <c r="B15" s="31"/>
+      <c r="B15" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
         <v>8</v>
@@ -6328,7 +6655,7 @@
         <v>9</v>
       </c>
       <c r="F15" s="7">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
@@ -6339,12 +6666,22 @@
       <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="7">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="7">
+        <v>14</v>
+      </c>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
@@ -6354,147 +6691,258 @@
       <c r="M16" s="19"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="7">
+        <v>11</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>41</v>
+      </c>
       <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="D17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="7">
+        <v>4</v>
+      </c>
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
+      <c r="I17" s="19">
+        <v>4</v>
+      </c>
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
     </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>12</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="7">
+        <v>4</v>
+      </c>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>13</v>
+      </c>
+      <c r="B19" s="43"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="7">
+        <v>4</v>
+      </c>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>14</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="7">
+        <v>4</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+    </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="12" t="s">
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="46"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+      <c r="B29" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="9" t="s">
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="11"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="7">
-        <f>COUNT(A7:A17)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
+      <c r="C31" s="7">
+        <f>COUNT(A7:A22)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C32" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C33" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B48" s="12" t="s">
+    <row r="53" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B53" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="15" t="s">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C55" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D55" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E55" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="7" t="s">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C56" s="7">
         <v>0</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D56" s="7">
         <v>0</v>
       </c>
-      <c r="E51" s="14" t="e">
-        <f>D51/C51</f>
+      <c r="E56" s="14" t="e">
+        <f>D56/C56</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="7" t="s">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C57" s="7">
         <v>0</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D57" s="7">
         <v>0</v>
       </c>
-      <c r="E52" s="14" t="e">
-        <f t="shared" ref="E52:E54" si="0">D52/C52</f>
+      <c r="E57" s="14" t="e">
+        <f t="shared" ref="E57:E59" si="0">D57/C57</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="7" t="s">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C58" s="7">
         <v>0</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D58" s="7">
         <v>0</v>
       </c>
-      <c r="E53" s="14" t="e">
+      <c r="E58" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="7" t="s">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C59" s="7">
         <v>0</v>
       </c>
-      <c r="D54" s="7">
+      <c r="D59" s="7">
         <v>0</v>
       </c>
-      <c r="E54" s="14" t="e">
+      <c r="E59" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -6502,9 +6950,9 @@
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="G5:M5"/>
-    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B17:B20"/>
     <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A21:C22"/>
+    <mergeCell ref="A26:C27"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="D5:D6"/>
@@ -6513,11 +6961,11 @@
     <mergeCell ref="A5:A6"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56:B59 D7:D22">
+      <formula1>Member</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E22">
       <formula1>Status</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51:B54 D7:D17">
-      <formula1>Member</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6525,7 +6973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M53"/>
   <sheetViews>
@@ -6544,11 +6992,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
@@ -6557,9 +7005,9 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
       <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
@@ -6568,41 +7016,41 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
       <c r="G6" s="5">
         <v>1</v>
       </c>
@@ -6796,16 +7244,16 @@
       <c r="M16" s="7"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -6951,7 +7399,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M53"/>
   <sheetViews>
@@ -6970,11 +7418,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
@@ -6983,9 +7431,9 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
       <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
@@ -6994,41 +7442,41 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
       <c r="G6" s="5">
         <v>1</v>
       </c>
@@ -7222,16 +7670,16 @@
       <c r="M16" s="7"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -7377,7 +7825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C10"/>
   <sheetViews>
@@ -7404,7 +7852,7 @@
       <c r="B5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="50" t="s">
         <v>8</v>
       </c>
     </row>
@@ -7415,7 +7863,7 @@
       <c r="B6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="50"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="22">
@@ -7424,7 +7872,7 @@
       <c r="B7" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="50" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7435,7 +7883,7 @@
       <c r="B8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="37"/>
+      <c r="C8" s="50"/>
     </row>
     <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
@@ -7469,7 +7917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -7502,7 +7950,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -7510,7 +7958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -7550,7 +7998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Review Report1, Update Backlog
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -1006,11 +1006,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="192920704"/>
-        <c:axId val="192921264"/>
+        <c:axId val="1888601152"/>
+        <c:axId val="1888604416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="192920704"/>
+        <c:axId val="1888601152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1053,7 +1053,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192921264"/>
+        <c:crossAx val="1888604416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1061,7 +1061,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="192921264"/>
+        <c:axId val="1888604416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1113,7 +1113,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192920704"/>
+        <c:crossAx val="1888601152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1594,11 +1594,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="192925184"/>
-        <c:axId val="192925744"/>
+        <c:axId val="1888589728"/>
+        <c:axId val="1888507024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="192925184"/>
+        <c:axId val="1888589728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1641,7 +1641,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192925744"/>
+        <c:crossAx val="1888507024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1649,7 +1649,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="192925744"/>
+        <c:axId val="1888507024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1701,7 +1701,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192925184"/>
+        <c:crossAx val="1888589728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2182,11 +2182,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="193881312"/>
-        <c:axId val="193881872"/>
+        <c:axId val="2039991872"/>
+        <c:axId val="2039992416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="193881312"/>
+        <c:axId val="2039991872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2229,7 +2229,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="193881872"/>
+        <c:crossAx val="2039992416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2237,7 +2237,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193881872"/>
+        <c:axId val="2039992416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2289,7 +2289,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="193881312"/>
+        <c:crossAx val="2039991872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6329,8 +6329,8 @@
   </sheetPr>
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
KhoaVNA - Update backlog
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="3030" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="10" r:id="rId1"/>
@@ -1006,11 +1006,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1888601152"/>
-        <c:axId val="1888604416"/>
+        <c:axId val="173029536"/>
+        <c:axId val="173030096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1888601152"/>
+        <c:axId val="173029536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1053,7 +1053,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888604416"/>
+        <c:crossAx val="173030096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1061,7 +1061,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1888604416"/>
+        <c:axId val="173030096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1113,7 +1113,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888601152"/>
+        <c:crossAx val="173029536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1594,11 +1594,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1888589728"/>
-        <c:axId val="1888507024"/>
+        <c:axId val="173034016"/>
+        <c:axId val="173034576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1888589728"/>
+        <c:axId val="173034016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1641,7 +1641,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888507024"/>
+        <c:crossAx val="173034576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1649,7 +1649,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1888507024"/>
+        <c:axId val="173034576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1701,7 +1701,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888589728"/>
+        <c:crossAx val="173034016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2182,11 +2182,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2039991872"/>
-        <c:axId val="2039992416"/>
+        <c:axId val="173038496"/>
+        <c:axId val="173039056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2039991872"/>
+        <c:axId val="173038496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2229,7 +2229,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2039992416"/>
+        <c:crossAx val="173039056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2237,7 +2237,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2039992416"/>
+        <c:axId val="173039056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2289,7 +2289,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2039991872"/>
+        <c:crossAx val="173038496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6329,8 +6329,8 @@
   </sheetPr>
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6668,7 +6668,9 @@
       <c r="J15" s="19">
         <v>5</v>
       </c>
-      <c r="K15" s="19"/>
+      <c r="K15" s="19">
+        <v>4</v>
+      </c>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
     </row>
@@ -6695,7 +6697,9 @@
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
+      <c r="K16" s="19">
+        <v>2</v>
+      </c>
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
     </row>

</xml_diff>

<commit_message>
Delete redundant files, Update Backlog
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -325,7 +325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -365,6 +365,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,7 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -551,6 +563,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -908,6 +930,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1009,11 +1032,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-873493008"/>
-        <c:axId val="-873502256"/>
+        <c:axId val="959967280"/>
+        <c:axId val="959969456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-873493008"/>
+        <c:axId val="959967280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1056,7 +1079,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-873502256"/>
+        <c:crossAx val="959969456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1064,7 +1087,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-873502256"/>
+        <c:axId val="959969456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1116,7 +1139,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-873493008"/>
+        <c:crossAx val="959967280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1597,11 +1620,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-873500624"/>
-        <c:axId val="-873500080"/>
+        <c:axId val="959971632"/>
+        <c:axId val="959968368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-873500624"/>
+        <c:axId val="959971632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1644,7 +1667,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-873500080"/>
+        <c:crossAx val="959968368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1652,7 +1675,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-873500080"/>
+        <c:axId val="959968368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1704,7 +1727,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-873500624"/>
+        <c:crossAx val="959971632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2185,11 +2208,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-720304032"/>
-        <c:axId val="-720304576"/>
+        <c:axId val="959970544"/>
+        <c:axId val="959965648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-720304032"/>
+        <c:axId val="959970544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2232,7 +2255,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-720304576"/>
+        <c:crossAx val="959965648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2240,7 +2263,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-720304576"/>
+        <c:axId val="959965648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2292,7 +2315,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-720304032"/>
+        <c:crossAx val="959970544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6333,7 +6356,7 @@
   <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6467,254 +6490,256 @@
         <v>5</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F8" s="7">
         <v>16</v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I8" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J8" s="19">
-        <v>6</v>
-      </c>
-      <c r="K8" s="19"/>
+        <v>5</v>
+      </c>
+      <c r="K8" s="19">
+        <v>2</v>
+      </c>
       <c r="L8" s="19"/>
       <c r="M8" s="19"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+    <row r="9" spans="1:13" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52">
         <v>3</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="52"/>
+      <c r="D9" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="52">
         <v>4</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
+    </row>
+    <row r="10" spans="1:13" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52">
         <v>4</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="52"/>
+      <c r="D10" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="52">
         <v>4</v>
       </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+    </row>
+    <row r="11" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="49">
         <v>5</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="49">
         <v>14</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="50">
         <v>5</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="50">
         <v>2</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="50">
         <v>2</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+    </row>
+    <row r="12" spans="1:13" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="52">
         <v>6</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="52">
         <v>14</v>
       </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+    </row>
+    <row r="13" spans="1:13" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="52">
         <v>7</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="52">
         <v>14</v>
       </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
+    </row>
+    <row r="14" spans="1:13" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="52">
         <v>8</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="52">
         <v>14</v>
       </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+    </row>
+    <row r="15" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="49">
         <v>9</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="7">
+      <c r="E15" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="49">
         <v>14</v>
       </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19">
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50">
         <v>4</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="50">
         <v>5</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="50">
         <v>4</v>
       </c>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+    </row>
+    <row r="16" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="49">
         <v>10</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="7">
+      <c r="E16" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="49">
         <v>14</v>
       </c>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19">
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50">
         <v>2</v>
       </c>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>76</v>
@@ -6743,30 +6768,32 @@
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>15</v>
-      </c>
-      <c r="B18" s="7" t="s">
+    <row r="18" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="49">
+        <v>12</v>
+      </c>
+      <c r="B18" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="49"/>
+      <c r="D18" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19">
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50">
         <v>2</v>
       </c>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
+      <c r="K18" s="50">
+        <v>2</v>
+      </c>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
@@ -6935,7 +6962,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update Report 2 + Backlog
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="5820" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBacklog" sheetId="11" r:id="rId1"/>
@@ -1182,11 +1182,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1627893136"/>
-        <c:axId val="-1627906192"/>
+        <c:axId val="156859328"/>
+        <c:axId val="156859888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1627893136"/>
+        <c:axId val="156859328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1229,7 +1229,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1627906192"/>
+        <c:crossAx val="156859888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1237,7 +1237,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1627906192"/>
+        <c:axId val="156859888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1289,7 +1289,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1627893136"/>
+        <c:crossAx val="156859328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1378,7 +1378,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1496,9 +1495,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1672,7 +1669,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1774,11 +1770,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1627904016"/>
-        <c:axId val="-1396030496"/>
+        <c:axId val="157797664"/>
+        <c:axId val="157798224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1627904016"/>
+        <c:axId val="157797664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1821,7 +1817,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1396030496"/>
+        <c:crossAx val="157798224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1829,7 +1825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1396030496"/>
+        <c:axId val="157798224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1881,7 +1877,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1627904016"/>
+        <c:crossAx val="157797664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2362,11 +2358,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1396032672"/>
-        <c:axId val="-1396023424"/>
+        <c:axId val="157802144"/>
+        <c:axId val="157802704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1396032672"/>
+        <c:axId val="157802144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2409,7 +2405,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1396023424"/>
+        <c:crossAx val="157802704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2417,7 +2413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1396023424"/>
+        <c:axId val="157802704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2469,7 +2465,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1396032672"/>
+        <c:crossAx val="157802144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6316,8 +6312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7380,8 +7376,8 @@
   </sheetPr>
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7681,14 +7677,20 @@
         <v>8</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F14" s="7">
         <v>12</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="G14" s="7">
+        <v>10</v>
+      </c>
+      <c r="H14" s="7">
+        <v>8</v>
+      </c>
+      <c r="I14" s="7">
+        <v>6</v>
+      </c>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -7738,9 +7740,15 @@
       <c r="F16" s="51">
         <v>8</v>
       </c>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="51"/>
+      <c r="G16" s="51">
+        <v>6</v>
+      </c>
+      <c r="H16" s="51">
+        <v>5</v>
+      </c>
+      <c r="I16" s="51">
+        <v>3</v>
+      </c>
       <c r="J16" s="51"/>
       <c r="K16" s="51"/>
       <c r="L16" s="51"/>

</xml_diff>